<commit_message>
Video Game Version 1.0
Finally the grand finale
All of the requirements have been met, proper coding practices have been
followed, everything works, movement is done via a matrix, I have gone
blind from staring at the computer, and I have drank more coffee in the
past week than in my whole life.
</commit_message>
<xml_diff>
--- a/Game Map.xlsx
+++ b/Game Map.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>(x,y)</t>
-  </si>
-  <si>
-    <t>START</t>
   </si>
 </sst>
 </file>
@@ -536,77 +533,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,7 +916,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,10 +938,10 @@
       <c r="D1" s="16">
         <v>2</v>
       </c>
-      <c r="E1" s="21">
+      <c r="E1" s="20">
         <v>3</v>
       </c>
-      <c r="F1" s="21">
+      <c r="F1" s="20">
         <v>4</v>
       </c>
       <c r="G1" s="3">
@@ -961,12 +958,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31" t="s">
+      <c r="C2" s="28">
+        <v>2</v>
+      </c>
+      <c r="D2" s="29">
         <v>1</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="E2" s="30">
+        <v>0</v>
+      </c>
+      <c r="F2" s="34">
+        <v>16</v>
+      </c>
       <c r="G2" s="11"/>
       <c r="H2" s="9"/>
       <c r="I2" s="15"/>
@@ -980,36 +983,60 @@
       <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="24"/>
+      <c r="B3" s="28">
+        <v>6</v>
+      </c>
+      <c r="C3" s="31">
+        <v>5</v>
+      </c>
+      <c r="D3" s="32">
+        <v>4</v>
+      </c>
+      <c r="E3" s="29">
+        <v>3</v>
+      </c>
+      <c r="F3" s="36">
+        <v>14</v>
+      </c>
+      <c r="G3" s="29">
+        <v>15</v>
+      </c>
+      <c r="H3" s="23"/>
       <c r="I3" s="15"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="38"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="28">
+        <v>7</v>
+      </c>
+      <c r="D4" s="33">
+        <v>8</v>
+      </c>
+      <c r="E4" s="35">
+        <v>10</v>
+      </c>
+      <c r="F4" s="33">
+        <v>11</v>
+      </c>
+      <c r="G4" s="35">
+        <v>12</v>
+      </c>
+      <c r="H4" s="37">
+        <v>13</v>
+      </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:15" ht="46.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1017,12 +1044,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="10"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="39"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="38">
+        <v>9</v>
+      </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="5"/>
@@ -1039,8 +1068,10 @@
       <c r="D6" s="7"/>
       <c r="E6" s="11"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="39">
+        <v>17</v>
+      </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="5"/>
@@ -1053,9 +1084,13 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="41"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="42">
+        <v>20</v>
+      </c>
+      <c r="H7" s="40">
+        <v>18</v>
+      </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="5"/>
@@ -1069,8 +1104,10 @@
       <c r="D8" s="7"/>
       <c r="E8" s="10"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="42"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="41">
+        <v>19</v>
+      </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="5"/>
@@ -1086,7 +1123,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="28"/>
+      <c r="H9" s="27"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>

</xml_diff>